<commit_message>
Added function to read instrument dates from xlsx rather than csv
</commit_message>
<xml_diff>
--- a/data/data_selection/data_release_schedule.xlsx
+++ b/data/data_selection/data_release_schedule.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chxmr/code/agage-archive/data/data_selection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD912E5A-38B9-5048-81EA-56B0685C9DCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{731DDBA8-FE35-984D-978C-5E13776AD3B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7500" yWindow="1500" windowWidth="27240" windowHeight="16440" xr2:uid="{D0121EA7-C121-5646-A290-A6B31742EFF2}"/>
+    <workbookView xWindow="7500" yWindow="1500" windowWidth="27240" windowHeight="16440" activeTab="1" xr2:uid="{D0121EA7-C121-5646-A290-A6B31742EFF2}"/>
   </bookViews>
   <sheets>
     <sheet name="GCMD" sheetId="1" r:id="rId1"/>
-    <sheet name="GC-ECD-SF6" sheetId="2" r:id="rId2"/>
+    <sheet name="GCECD" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="38">
   <si>
     <t>CFC-11</t>
   </si>
@@ -546,8 +546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F54C872C-8629-284F-A579-6B1D027BD782}">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -745,95 +745,66 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45B7D617-534A-7D4D-B320-EB699FEFA4E5}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20" style="1" customWidth="1"/>
-    <col min="2" max="4" width="15.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.1640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>34</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F9" s="1" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Individual instruments now run for ALE/GAGE/GCMD/GCMS-
</commit_message>
<xml_diff>
--- a/data/data_selection/data_release_schedule.xlsx
+++ b/data/data_selection/data_release_schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chxmr/code/agage-archive/data/data_selection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12183BAA-2DFA-3D4E-A5F9-D8B73724319C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1049773-3D80-9549-859F-2DB3E04EC8BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="760" windowWidth="27240" windowHeight="16440" activeTab="5" xr2:uid="{D0121EA7-C121-5646-A290-A6B31742EFF2}"/>
+    <workbookView xWindow="960" yWindow="760" windowWidth="27240" windowHeight="16440" activeTab="4" xr2:uid="{D0121EA7-C121-5646-A290-A6B31742EFF2}"/>
   </bookViews>
   <sheets>
     <sheet name="GAGE" sheetId="7" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="87">
   <si>
     <t>MHD</t>
   </si>
@@ -228,9 +228,6 @@
   </si>
   <si>
     <t>GSN</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t xml:space="preserve">x </t>
@@ -431,7 +428,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -463,30 +460,43 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -861,7 +871,7 @@
         <v>0</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>2</v>
@@ -907,7 +917,7 @@
       <c r="A15" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="16"/>
+      <c r="B15" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1506,1050 +1516,984 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CEEAF2A-BA72-FC4F-92D8-D72395398919}">
   <dimension ref="A1:J63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20" style="17" customWidth="1"/>
-    <col min="2" max="10" width="19" style="17" customWidth="1"/>
-    <col min="11" max="16384" width="10.83203125" style="18"/>
+    <col min="1" max="1" width="20" style="18" customWidth="1"/>
+    <col min="2" max="10" width="19" style="18" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-    </row>
-    <row r="2" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="17" t="s">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-    </row>
-    <row r="3" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="17" t="s">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-    </row>
-    <row r="4" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="17" t="s">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
-    </row>
-    <row r="5" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="17" t="s">
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="17"/>
-    </row>
-    <row r="6" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="17" t="s">
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
-    </row>
-    <row r="7" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="19" t="s">
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="17"/>
-    </row>
-    <row r="8" spans="1:10" s="18" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="20" t="s">
+    </row>
+    <row r="8" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D8" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="21" t="s">
+      <c r="E8" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="21" t="s">
+      <c r="F8" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="21" t="s">
+      <c r="G8" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="H8" s="21" t="s">
+      <c r="H8" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="I8" s="21" t="s">
+      <c r="I8" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="J8" s="21" t="s">
+      <c r="J8" s="22" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="18" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="22" t="s">
+    <row r="9" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="J9" s="23" t="s">
+      <c r="B9" s="23"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="J9" s="24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="B10" s="23"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="23"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="23"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="B13" s="23"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="23"/>
+      <c r="I13" s="23"/>
+      <c r="J13" s="24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="23"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" s="23"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" s="23"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="24"/>
+      <c r="J16" s="24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="23"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="23"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" s="23"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="23"/>
+      <c r="I18" s="23"/>
+      <c r="J18" s="24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="B19" s="25"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="25"/>
+      <c r="I19" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="J19" s="26" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="25"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="26"/>
+      <c r="H20" s="24" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" s="18" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="22" t="s">
-        <v>70</v>
-      </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="23" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" s="18" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="23" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" s="18" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="23" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" s="18" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="23" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" s="18" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="23" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" s="18" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="23" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" s="18" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="23"/>
-      <c r="J16" s="23" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" s="18" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="B17" s="15"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="15"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="23" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" s="18" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="B18" s="15"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="23" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" s="18" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A19" s="24" t="s">
+      <c r="I20" s="25"/>
+      <c r="J20" s="26" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="J19" s="25" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" s="18" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="25" t="s">
+      <c r="B21" s="25"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="25"/>
+      <c r="I21" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="J21" s="26" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="B22" s="25"/>
+      <c r="C22" s="25"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="25"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="25"/>
+      <c r="H22" s="25"/>
+      <c r="I22" s="25"/>
+      <c r="J22" s="24" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="B23" s="25"/>
+      <c r="C23" s="25"/>
+      <c r="D23" s="25"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="25"/>
+      <c r="G23" s="25"/>
+      <c r="H23" s="25"/>
+      <c r="I23" s="25"/>
+      <c r="J23" s="24" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" s="25"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="25"/>
+      <c r="H24" s="25"/>
+      <c r="I24" s="25"/>
+      <c r="J24" s="26" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" s="25"/>
+      <c r="C25" s="25"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="25"/>
+      <c r="H25" s="25"/>
+      <c r="I25" s="25"/>
+      <c r="J25" s="24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C26" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F26" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="G26" s="25"/>
+      <c r="H26" s="25"/>
+      <c r="I26" s="25"/>
+      <c r="J26" s="24" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="D27" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="E27" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F27" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="G27" s="25"/>
+      <c r="H27" s="25"/>
+      <c r="I27" s="25"/>
+      <c r="J27" s="24" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="J28" s="24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B29" s="25"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="25"/>
+      <c r="F29" s="25"/>
+      <c r="G29" s="25"/>
+      <c r="H29" s="25"/>
+      <c r="I29" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="J29" s="24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="B30" s="25"/>
+      <c r="C30" s="25"/>
+      <c r="D30" s="25"/>
+      <c r="E30" s="25"/>
+      <c r="F30" s="25"/>
+      <c r="G30" s="25"/>
+      <c r="H30" s="25"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="B31" s="25"/>
+      <c r="C31" s="25"/>
+      <c r="D31" s="25"/>
+      <c r="E31" s="25"/>
+      <c r="F31" s="25"/>
+      <c r="G31" s="25"/>
+      <c r="H31" s="25"/>
+      <c r="I31" s="26"/>
+      <c r="J31" s="24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A32" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="B32" s="25"/>
+      <c r="C32" s="25"/>
+      <c r="D32" s="25"/>
+      <c r="E32" s="25"/>
+      <c r="F32" s="25"/>
+      <c r="G32" s="25"/>
+      <c r="H32" s="25"/>
+      <c r="I32" s="25"/>
+      <c r="J32" s="24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A33" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B33" s="25"/>
+      <c r="C33" s="25"/>
+      <c r="D33" s="25"/>
+      <c r="E33" s="25"/>
+      <c r="F33" s="25"/>
+      <c r="G33" s="25"/>
+      <c r="H33" s="25"/>
+      <c r="I33" s="25"/>
+      <c r="J33" s="24" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A34" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="B34" s="25"/>
+      <c r="C34" s="25"/>
+      <c r="D34" s="25"/>
+      <c r="E34" s="25"/>
+      <c r="F34" s="25"/>
+      <c r="G34" s="25"/>
+      <c r="H34" s="25"/>
+      <c r="I34" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="J34" s="24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A35" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B35" s="25"/>
+      <c r="C35" s="25"/>
+      <c r="D35" s="25"/>
+      <c r="E35" s="25"/>
+      <c r="F35" s="25"/>
+      <c r="G35" s="25"/>
+      <c r="H35" s="25"/>
+      <c r="I35" s="25"/>
+      <c r="J35" s="24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A36" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B36" s="25"/>
+      <c r="C36" s="25"/>
+      <c r="D36" s="25"/>
+      <c r="E36" s="25"/>
+      <c r="F36" s="25"/>
+      <c r="G36" s="25"/>
+      <c r="H36" s="25"/>
+      <c r="I36" s="25"/>
+      <c r="J36" s="24" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A37" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B37" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="C37" s="25"/>
+      <c r="D37" s="25"/>
+      <c r="E37" s="25"/>
+      <c r="F37" s="25"/>
+      <c r="G37" s="25"/>
+      <c r="H37" s="25"/>
+      <c r="I37" s="25"/>
+      <c r="J37" s="26" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A38" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="C38" s="25"/>
+      <c r="D38" s="25"/>
+      <c r="E38" s="25"/>
+      <c r="F38" s="25"/>
+      <c r="G38" s="25"/>
+      <c r="H38" s="25"/>
+      <c r="I38" s="25"/>
+      <c r="J38" s="24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A39" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B39" s="25"/>
+      <c r="C39" s="25"/>
+      <c r="D39" s="25"/>
+      <c r="E39" s="25"/>
+      <c r="F39" s="25"/>
+      <c r="G39" s="25"/>
+      <c r="H39" s="25"/>
+      <c r="I39" s="25"/>
+      <c r="J39" s="24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A40" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B40" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C40" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="D40" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="E40" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F40" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="G40" s="25"/>
+      <c r="H40" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="I40" s="25"/>
+      <c r="J40" s="24" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A41" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="B41" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="H20" s="23" t="s">
+      <c r="C41" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="D41" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="E41" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F41" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="G41" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="H41" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="I41" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="J41" s="26" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A42" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="B42" s="25"/>
+      <c r="C42" s="25"/>
+      <c r="D42" s="26"/>
+      <c r="E42" s="25"/>
+      <c r="F42" s="25"/>
+      <c r="G42" s="25"/>
+      <c r="H42" s="25"/>
+      <c r="I42" s="25"/>
+      <c r="J42" s="26" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A43" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B43" s="25"/>
+      <c r="C43" s="25"/>
+      <c r="D43" s="25"/>
+      <c r="E43" s="25"/>
+      <c r="F43" s="25"/>
+      <c r="G43" s="25"/>
+      <c r="H43" s="25"/>
+      <c r="I43" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="J43" s="24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A44" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="B44" s="25"/>
+      <c r="C44" s="25"/>
+      <c r="D44" s="25"/>
+      <c r="E44" s="25"/>
+      <c r="F44" s="25"/>
+      <c r="G44" s="25"/>
+      <c r="H44" s="25"/>
+      <c r="I44" s="25"/>
+      <c r="J44" s="26" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A45" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="B45" s="25"/>
+      <c r="C45" s="25"/>
+      <c r="D45" s="25"/>
+      <c r="E45" s="25"/>
+      <c r="F45" s="25"/>
+      <c r="G45" s="25"/>
+      <c r="H45" s="25"/>
+      <c r="I45" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="J45" s="26" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A46" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="B46" s="25"/>
+      <c r="C46" s="25"/>
+      <c r="D46" s="25"/>
+      <c r="E46" s="25"/>
+      <c r="F46" s="25"/>
+      <c r="G46" s="25"/>
+      <c r="H46" s="25"/>
+      <c r="I46" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="J46" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="I20" s="9"/>
-      <c r="J20" s="25" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" s="18" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="24" t="s">
-        <v>73</v>
-      </c>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="J21" s="25" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" s="18" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" s="24" t="s">
-        <v>74</v>
-      </c>
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
-      <c r="J22" s="23" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" s="18" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="B23" s="9"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="23" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" s="18" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A24" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
-      <c r="J24" s="25" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" s="18" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A25" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="B25" s="9"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="9"/>
-      <c r="I25" s="9"/>
-      <c r="J25" s="23" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" s="18" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A26" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="B26" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="C26" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="D26" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="E26" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="F26" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="G26" s="9"/>
-      <c r="H26" s="9"/>
-      <c r="I26" s="9"/>
-      <c r="J26" s="23" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" s="18" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A27" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="B27" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="C27" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="D27" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="E27" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="F27" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="G27" s="9"/>
-      <c r="H27" s="9"/>
-      <c r="I27" s="9"/>
-      <c r="J27" s="23" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" s="18" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A28" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="B28" s="9"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="9"/>
-      <c r="H28" s="9"/>
-      <c r="I28" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="J28" s="23" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" s="18" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A29" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="B29" s="9"/>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9"/>
-      <c r="H29" s="9"/>
-      <c r="I29" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="J29" s="23" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" s="18" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A30" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="B30" s="9"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
-      <c r="H30" s="9"/>
-      <c r="I30" s="25"/>
-      <c r="J30" s="23" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" s="18" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="B31" s="9"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="9"/>
-      <c r="I31" s="25"/>
-      <c r="J31" s="23" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" s="18" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A32" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="B32" s="9"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="9"/>
-      <c r="G32" s="9"/>
-      <c r="H32" s="9"/>
-      <c r="I32" s="9"/>
-      <c r="J32" s="23" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" s="18" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A33" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="B33" s="9"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="9"/>
-      <c r="H33" s="9"/>
-      <c r="I33" s="9"/>
-      <c r="J33" s="23" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" s="18" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A34" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="B34" s="9"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="9"/>
-      <c r="G34" s="9"/>
-      <c r="H34" s="9"/>
-      <c r="I34" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="J34" s="23" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" s="18" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A35" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="B35" s="9"/>
-      <c r="C35" s="9"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="9"/>
-      <c r="H35" s="9"/>
-      <c r="I35" s="9"/>
-      <c r="J35" s="23" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" s="18" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A36" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="B36" s="9"/>
-      <c r="C36" s="9"/>
-      <c r="D36" s="9"/>
-      <c r="E36" s="9"/>
-      <c r="F36" s="9"/>
-      <c r="G36" s="9"/>
-      <c r="H36" s="9"/>
-      <c r="I36" s="9"/>
-      <c r="J36" s="23" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" s="18" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A37" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="B37" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="C37" s="9"/>
-      <c r="D37" s="9"/>
-      <c r="E37" s="9"/>
-      <c r="F37" s="9"/>
-      <c r="G37" s="9"/>
-      <c r="H37" s="9"/>
-      <c r="I37" s="9"/>
-      <c r="J37" s="25" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" s="18" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A38" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="B38" s="23" t="s">
-        <v>69</v>
-      </c>
-      <c r="C38" s="9"/>
-      <c r="D38" s="9"/>
-      <c r="E38" s="9"/>
-      <c r="F38" s="9"/>
-      <c r="G38" s="9"/>
-      <c r="H38" s="9"/>
-      <c r="I38" s="9"/>
-      <c r="J38" s="23" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" s="18" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A39" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="B39" s="9"/>
-      <c r="C39" s="9"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="9"/>
-      <c r="F39" s="9"/>
-      <c r="G39" s="9"/>
-      <c r="H39" s="9"/>
-      <c r="I39" s="9"/>
-      <c r="J39" s="23" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" s="18" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A40" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="B40" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="C40" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="D40" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="E40" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="F40" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="G40" s="9"/>
-      <c r="H40" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="I40" s="9"/>
-      <c r="J40" s="23" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" s="18" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A41" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="B41" s="25" t="s">
+    </row>
+    <row r="47" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A47" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="B47" s="25"/>
+      <c r="C47" s="25"/>
+      <c r="D47" s="25"/>
+      <c r="E47" s="25"/>
+      <c r="F47" s="25"/>
+      <c r="G47" s="25"/>
+      <c r="H47" s="25"/>
+      <c r="I47" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="J47" s="24" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A48" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="B48" s="25"/>
+      <c r="C48" s="25"/>
+      <c r="D48" s="25"/>
+      <c r="E48" s="25"/>
+      <c r="F48" s="25"/>
+      <c r="G48" s="25"/>
+      <c r="H48" s="25"/>
+      <c r="I48" s="25"/>
+      <c r="J48" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="C41" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="D41" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="E41" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="F41" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="G41" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="H41" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="I41" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="J41" s="25" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" s="18" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A42" s="24" t="s">
-        <v>54</v>
-      </c>
-      <c r="B42" s="9"/>
-      <c r="C42" s="9"/>
-      <c r="D42" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="E42" s="9"/>
-      <c r="F42" s="9"/>
-      <c r="G42" s="9"/>
-      <c r="H42" s="9"/>
-      <c r="I42" s="9"/>
-      <c r="J42" s="25" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" s="18" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A43" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="B43" s="9"/>
-      <c r="C43" s="9"/>
-      <c r="D43" s="9"/>
-      <c r="E43" s="9"/>
-      <c r="F43" s="9"/>
-      <c r="G43" s="9"/>
-      <c r="H43" s="9"/>
-      <c r="I43" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="J43" s="23" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" s="18" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A44" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="B44" s="9"/>
-      <c r="C44" s="9"/>
-      <c r="D44" s="9"/>
-      <c r="E44" s="9"/>
-      <c r="F44" s="9"/>
-      <c r="G44" s="9"/>
-      <c r="H44" s="9"/>
-      <c r="I44" s="9"/>
-      <c r="J44" s="25" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" s="18" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A45" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="B45" s="9"/>
-      <c r="C45" s="9"/>
-      <c r="D45" s="9"/>
-      <c r="E45" s="9"/>
-      <c r="F45" s="9"/>
-      <c r="G45" s="9"/>
-      <c r="H45" s="9"/>
-      <c r="I45" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="J45" s="25" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" s="18" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A46" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="B46" s="9"/>
-      <c r="C46" s="9"/>
-      <c r="D46" s="9"/>
-      <c r="E46" s="9"/>
-      <c r="F46" s="9"/>
-      <c r="G46" s="9"/>
-      <c r="H46" s="9"/>
-      <c r="I46" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="J46" s="23" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" s="18" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A47" s="24" t="s">
-        <v>82</v>
-      </c>
-      <c r="B47" s="9"/>
-      <c r="C47" s="9"/>
-      <c r="D47" s="9"/>
-      <c r="E47" s="9"/>
-      <c r="F47" s="9"/>
-      <c r="G47" s="9"/>
-      <c r="H47" s="9"/>
-      <c r="I47" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="J47" s="23" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" s="18" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A48" s="24" t="s">
+    </row>
+    <row r="49" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A49" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="B48" s="9"/>
-      <c r="C48" s="9"/>
-      <c r="D48" s="9"/>
-      <c r="E48" s="9"/>
-      <c r="F48" s="9"/>
-      <c r="G48" s="9"/>
-      <c r="H48" s="9"/>
-      <c r="I48" s="9"/>
-      <c r="J48" s="23" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" s="18" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A49" s="24" t="s">
-        <v>84</v>
-      </c>
-      <c r="B49" s="9"/>
-      <c r="C49" s="9"/>
-      <c r="D49" s="9"/>
-      <c r="E49" s="9"/>
-      <c r="F49" s="9"/>
-      <c r="G49" s="9"/>
-      <c r="H49" s="9"/>
-      <c r="I49" s="9"/>
-      <c r="J49" s="23" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="26"/>
-      <c r="B50" s="26"/>
-      <c r="C50" s="26"/>
-      <c r="D50" s="26"/>
-      <c r="E50" s="26"/>
-      <c r="F50" s="26"/>
-      <c r="G50" s="26"/>
-      <c r="H50" s="26"/>
-      <c r="I50" s="26"/>
-      <c r="J50" s="26"/>
-    </row>
-    <row r="51" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="26"/>
-      <c r="B51" s="26"/>
-      <c r="C51" s="26"/>
-      <c r="D51" s="26"/>
-      <c r="E51" s="26"/>
-      <c r="F51" s="26"/>
-      <c r="G51" s="26"/>
-      <c r="H51" s="26"/>
-      <c r="I51" s="26"/>
-      <c r="J51" s="26"/>
-    </row>
-    <row r="52" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="26"/>
-      <c r="B52" s="26"/>
-      <c r="C52" s="26"/>
-      <c r="D52" s="26"/>
-      <c r="E52" s="26"/>
-      <c r="F52" s="26"/>
-      <c r="G52" s="26"/>
-      <c r="H52" s="26"/>
-      <c r="I52" s="26"/>
-      <c r="J52" s="26"/>
-    </row>
-    <row r="53" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="26"/>
-      <c r="B53" s="26"/>
-      <c r="C53" s="26"/>
-      <c r="D53" s="26"/>
-      <c r="E53" s="26"/>
-      <c r="F53" s="26"/>
-      <c r="G53" s="26"/>
-      <c r="H53" s="26"/>
-      <c r="I53" s="26"/>
-      <c r="J53" s="26"/>
-    </row>
-    <row r="54" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="26"/>
-      <c r="B54" s="26"/>
-      <c r="C54" s="26"/>
-      <c r="D54" s="26"/>
-      <c r="E54" s="26"/>
-      <c r="F54" s="26"/>
-      <c r="G54" s="26"/>
-      <c r="H54" s="26"/>
-      <c r="I54" s="26"/>
-      <c r="J54" s="26"/>
-    </row>
-    <row r="55" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="26"/>
-      <c r="B55" s="26"/>
-      <c r="C55" s="26"/>
-      <c r="D55" s="26"/>
-      <c r="E55" s="26"/>
-      <c r="F55" s="26"/>
-      <c r="G55" s="26"/>
-      <c r="H55" s="26"/>
-      <c r="I55" s="26"/>
-      <c r="J55" s="26"/>
-    </row>
-    <row r="56" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="26"/>
-      <c r="B56" s="26"/>
-      <c r="C56" s="26"/>
-      <c r="D56" s="26"/>
-      <c r="E56" s="26"/>
-      <c r="F56" s="26"/>
-      <c r="G56" s="26"/>
-      <c r="H56" s="26"/>
-      <c r="I56" s="26"/>
-      <c r="J56" s="26"/>
-    </row>
-    <row r="57" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="26"/>
-      <c r="B57" s="26"/>
-      <c r="C57" s="26"/>
-      <c r="D57" s="26"/>
-      <c r="E57" s="26"/>
-      <c r="F57" s="26"/>
-      <c r="G57" s="26"/>
-      <c r="H57" s="26"/>
-      <c r="I57" s="26"/>
-      <c r="J57" s="26"/>
-    </row>
-    <row r="58" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="26"/>
-      <c r="B58" s="26"/>
-      <c r="C58" s="26"/>
-      <c r="D58" s="26"/>
-      <c r="E58" s="26"/>
-      <c r="F58" s="26"/>
-      <c r="G58" s="26"/>
-      <c r="H58" s="26"/>
-      <c r="I58" s="26"/>
-      <c r="J58" s="26"/>
-    </row>
-    <row r="59" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="26"/>
-      <c r="B59" s="26"/>
-      <c r="C59" s="26"/>
-      <c r="D59" s="26"/>
-      <c r="E59" s="26"/>
-      <c r="F59" s="26"/>
-      <c r="G59" s="26"/>
-      <c r="H59" s="26"/>
-      <c r="I59" s="26"/>
-      <c r="J59" s="26"/>
-    </row>
-    <row r="60" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="26"/>
-      <c r="B60" s="26"/>
-      <c r="C60" s="26"/>
-      <c r="D60" s="26"/>
-      <c r="E60" s="26"/>
-      <c r="F60" s="26"/>
-      <c r="G60" s="26"/>
-      <c r="H60" s="26"/>
-      <c r="I60" s="26"/>
-      <c r="J60" s="26"/>
-    </row>
-    <row r="61" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="26"/>
-      <c r="B61" s="26"/>
-      <c r="C61" s="26"/>
-      <c r="D61" s="26"/>
-      <c r="E61" s="26"/>
-      <c r="F61" s="26"/>
-      <c r="G61" s="26"/>
-      <c r="H61" s="26"/>
-      <c r="I61" s="26"/>
-      <c r="J61" s="26"/>
-    </row>
-    <row r="62" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="26"/>
-      <c r="B62" s="26"/>
-      <c r="C62" s="26"/>
-      <c r="D62" s="26"/>
-      <c r="E62" s="26"/>
-      <c r="F62" s="26"/>
-      <c r="G62" s="26"/>
-      <c r="H62" s="26"/>
-      <c r="I62" s="26"/>
-      <c r="J62" s="26"/>
-    </row>
-    <row r="63" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="26"/>
-      <c r="B63" s="26"/>
-      <c r="C63" s="26"/>
-      <c r="D63" s="26"/>
-      <c r="E63" s="26"/>
-      <c r="F63" s="26"/>
-      <c r="G63" s="26"/>
-      <c r="H63" s="26"/>
-      <c r="I63" s="26"/>
-      <c r="J63" s="26"/>
+      <c r="B49" s="25"/>
+      <c r="C49" s="25"/>
+      <c r="D49" s="25"/>
+      <c r="E49" s="25"/>
+      <c r="F49" s="25"/>
+      <c r="G49" s="25"/>
+      <c r="H49" s="25"/>
+      <c r="I49" s="25"/>
+      <c r="J49" s="24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A50" s="27"/>
+      <c r="B50" s="27"/>
+      <c r="C50" s="27"/>
+      <c r="D50" s="27"/>
+      <c r="E50" s="27"/>
+      <c r="F50" s="27"/>
+      <c r="G50" s="27"/>
+      <c r="H50" s="27"/>
+      <c r="I50" s="27"/>
+      <c r="J50" s="27"/>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A51" s="27"/>
+      <c r="B51" s="27"/>
+      <c r="C51" s="27"/>
+      <c r="D51" s="27"/>
+      <c r="E51" s="27"/>
+      <c r="F51" s="27"/>
+      <c r="G51" s="27"/>
+      <c r="H51" s="27"/>
+      <c r="I51" s="27"/>
+      <c r="J51" s="27"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A52" s="27"/>
+      <c r="B52" s="27"/>
+      <c r="C52" s="27"/>
+      <c r="D52" s="27"/>
+      <c r="E52" s="27"/>
+      <c r="F52" s="27"/>
+      <c r="G52" s="27"/>
+      <c r="H52" s="27"/>
+      <c r="I52" s="27"/>
+      <c r="J52" s="27"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A53" s="27"/>
+      <c r="B53" s="27"/>
+      <c r="C53" s="27"/>
+      <c r="D53" s="27"/>
+      <c r="E53" s="27"/>
+      <c r="F53" s="27"/>
+      <c r="G53" s="27"/>
+      <c r="H53" s="27"/>
+      <c r="I53" s="27"/>
+      <c r="J53" s="27"/>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A54" s="27"/>
+      <c r="B54" s="27"/>
+      <c r="C54" s="27"/>
+      <c r="D54" s="27"/>
+      <c r="E54" s="27"/>
+      <c r="F54" s="27"/>
+      <c r="G54" s="27"/>
+      <c r="H54" s="27"/>
+      <c r="I54" s="27"/>
+      <c r="J54" s="27"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A55" s="27"/>
+      <c r="B55" s="27"/>
+      <c r="C55" s="27"/>
+      <c r="D55" s="27"/>
+      <c r="E55" s="27"/>
+      <c r="F55" s="27"/>
+      <c r="G55" s="27"/>
+      <c r="H55" s="27"/>
+      <c r="I55" s="27"/>
+      <c r="J55" s="27"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A56" s="27"/>
+      <c r="B56" s="27"/>
+      <c r="C56" s="27"/>
+      <c r="D56" s="27"/>
+      <c r="E56" s="27"/>
+      <c r="F56" s="27"/>
+      <c r="G56" s="27"/>
+      <c r="H56" s="27"/>
+      <c r="I56" s="27"/>
+      <c r="J56" s="27"/>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A57" s="27"/>
+      <c r="B57" s="27"/>
+      <c r="C57" s="27"/>
+      <c r="D57" s="27"/>
+      <c r="E57" s="27"/>
+      <c r="F57" s="27"/>
+      <c r="G57" s="27"/>
+      <c r="H57" s="27"/>
+      <c r="I57" s="27"/>
+      <c r="J57" s="27"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A58" s="27"/>
+      <c r="B58" s="27"/>
+      <c r="C58" s="27"/>
+      <c r="D58" s="27"/>
+      <c r="E58" s="27"/>
+      <c r="F58" s="27"/>
+      <c r="G58" s="27"/>
+      <c r="H58" s="27"/>
+      <c r="I58" s="27"/>
+      <c r="J58" s="27"/>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A59" s="27"/>
+      <c r="B59" s="27"/>
+      <c r="C59" s="27"/>
+      <c r="D59" s="27"/>
+      <c r="E59" s="27"/>
+      <c r="F59" s="27"/>
+      <c r="G59" s="27"/>
+      <c r="H59" s="27"/>
+      <c r="I59" s="27"/>
+      <c r="J59" s="27"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A60" s="27"/>
+      <c r="B60" s="27"/>
+      <c r="C60" s="27"/>
+      <c r="D60" s="27"/>
+      <c r="E60" s="27"/>
+      <c r="F60" s="27"/>
+      <c r="G60" s="27"/>
+      <c r="H60" s="27"/>
+      <c r="I60" s="27"/>
+      <c r="J60" s="27"/>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A61" s="27"/>
+      <c r="B61" s="27"/>
+      <c r="C61" s="27"/>
+      <c r="D61" s="27"/>
+      <c r="E61" s="27"/>
+      <c r="F61" s="27"/>
+      <c r="G61" s="27"/>
+      <c r="H61" s="27"/>
+      <c r="I61" s="27"/>
+      <c r="J61" s="27"/>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A62" s="27"/>
+      <c r="B62" s="27"/>
+      <c r="C62" s="27"/>
+      <c r="D62" s="27"/>
+      <c r="E62" s="27"/>
+      <c r="F62" s="27"/>
+      <c r="G62" s="27"/>
+      <c r="H62" s="27"/>
+      <c r="I62" s="27"/>
+      <c r="J62" s="27"/>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A63" s="27"/>
+      <c r="B63" s="27"/>
+      <c r="C63" s="27"/>
+      <c r="D63" s="27"/>
+      <c r="E63" s="27"/>
+      <c r="F63" s="27"/>
+      <c r="G63" s="27"/>
+      <c r="H63" s="27"/>
+      <c r="I63" s="27"/>
+      <c r="J63" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2560,7 +2504,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70B19699-4EA0-E64B-B1C3-62F7D3FC418D}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
@@ -2685,10 +2629,10 @@
         <v>23</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>87</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
Now runs all instruments apart from PDD
</commit_message>
<xml_diff>
--- a/data/data_selection/data_release_schedule.xlsx
+++ b/data/data_selection/data_release_schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chxmr/code/agage-archive/data/data_selection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDD30E85-88D9-874D-93B4-9C9A54BA66CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF469934-C207-5D4B-96C0-B033955034C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18580" yWindow="500" windowWidth="27240" windowHeight="16440" activeTab="7" xr2:uid="{D0121EA7-C121-5646-A290-A6B31742EFF2}"/>
+    <workbookView xWindow="0" yWindow="1200" windowWidth="27240" windowHeight="16440" activeTab="7" xr2:uid="{D0121EA7-C121-5646-A290-A6B31742EFF2}"/>
   </bookViews>
   <sheets>
     <sheet name="GAGE" sheetId="7" r:id="rId1"/>
@@ -42,8 +42,26 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={4E5E7B0D-B6A0-8246-B428-30A869DD781A}</author>
+  </authors>
+  <commentList>
+    <comment ref="B12" authorId="0" shapeId="0" xr:uid="{4E5E7B0D-B6A0-8246-B428-30A869DD781A}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Removing this for now, because I can’t handle having the same species on two different Picarros</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="89">
   <si>
     <t>MHD</t>
   </si>
@@ -285,9 +303,6 @@
     <t>nf3</t>
   </si>
   <si>
-    <t>pfc-14</t>
-  </si>
-  <si>
     <t>pfc-116</t>
   </si>
   <si>
@@ -310,13 +325,16 @@
   </si>
   <si>
     <t>13co2</t>
+  </si>
+  <si>
+    <t>cf4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -355,6 +373,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -519,6 +543,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Matthew Rigby" id="{60FAC528-71CC-9C47-92F6-AF7323BA56B4}" userId="S::chxmr@bristol.ac.uk::ca6cd915-32ac-44b1-8565-a73cfd7038de" providerId="AD"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -816,6 +846,14 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="B12" dT="2023-07-28T09:57:58.28" personId="{60FAC528-71CC-9C47-92F6-AF7323BA56B4}" id="{4E5E7B0D-B6A0-8246-B428-30A869DD781A}">
+    <text>Removing this for now, because I can’t handle having the same species on two different Picarros</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{216712D6-F759-CF40-AD40-8084674EE526}">
   <dimension ref="A1:F15"/>
@@ -878,7 +916,7 @@
         <v>0</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>2</v>
@@ -1523,8 +1561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CEEAF2A-BA72-FC4F-92D8-D72395398919}">
   <dimension ref="A1:J63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2038,7 +2076,7 @@
     </row>
     <row r="34" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B34" s="25"/>
       <c r="C34" s="25"/>
@@ -2268,7 +2306,7 @@
     </row>
     <row r="46" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="17" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="B46" s="25"/>
       <c r="C46" s="25"/>
@@ -2286,7 +2324,7 @@
     </row>
     <row r="47" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B47" s="25"/>
       <c r="C47" s="25"/>
@@ -2304,7 +2342,7 @@
     </row>
     <row r="48" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B48" s="25"/>
       <c r="C48" s="25"/>
@@ -2320,7 +2358,7 @@
     </row>
     <row r="49" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B49" s="25"/>
       <c r="C49" s="25"/>
@@ -2636,10 +2674,10 @@
         <v>23</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>85</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>86</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>2</v>
@@ -2682,7 +2720,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B5DB9A0-5433-FF47-BABC-7C9213421903}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B5DB9A0-5433-FF47-BABC-7C9213421903}">
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -2753,7 +2791,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -2765,18 +2803,37 @@
       <c r="A11" s="5" t="s">
         <v>36</v>
       </c>
+      <c r="B11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>39</v>
       </c>
+      <c r="B12" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Completed comparison with Ray Wang's files. Updated data_exclude
</commit_message>
<xml_diff>
--- a/data/data_selection/data_release_schedule.xlsx
+++ b/data/data_selection/data_release_schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chxmr/code/agage-archive/data/data_selection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6A1F0BD-FA49-1847-8350-0DC1994AEEF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F6EE43D-37AF-A740-82B5-045A11D9343A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1200" windowWidth="27240" windowHeight="16440" activeTab="8" xr2:uid="{D0121EA7-C121-5646-A290-A6B31742EFF2}"/>
   </bookViews>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="88">
   <si>
     <t>MHD</t>
   </si>
@@ -341,7 +341,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -380,12 +380,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -969,7 +963,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:A15"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2896,7 +2890,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3000,10 +2994,16 @@
       <c r="A13" s="5" t="s">
         <v>86</v>
       </c>
+      <c r="B13" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="C13" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changed PFC output names to chemical formulae. Several datasets are removed from release schedule, while I figure out how to handle scale conversions
</commit_message>
<xml_diff>
--- a/data/data_selection/data_release_schedule.xlsx
+++ b/data/data_selection/data_release_schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chxmr/code/agage-archive/data/data_selection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F6EE43D-37AF-A740-82B5-045A11D9343A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B74C7AD6-0306-EB46-8977-1D59EEB704AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1200" windowWidth="27240" windowHeight="16440" activeTab="8" xr2:uid="{D0121EA7-C121-5646-A290-A6B31742EFF2}"/>
+    <workbookView xWindow="740" yWindow="1760" windowWidth="27240" windowHeight="16440" activeTab="8" xr2:uid="{D0121EA7-C121-5646-A290-A6B31742EFF2}"/>
   </bookViews>
   <sheets>
     <sheet name="ALE" sheetId="6" r:id="rId1"/>
@@ -46,11 +46,86 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>tc={E3A1BF50-0BC7-1141-AFC5-6E9E0F0C2A71}</author>
-    <author>tc={4E5E7B0D-B6A0-8246-B428-30A869DD781A}</author>
+    <author>tc={3918FDDB-A3E4-0B49-9E30-91DC8C33B5FA}</author>
   </authors>
   <commentList>
-    <comment ref="C10" authorId="0" shapeId="0" xr:uid="{E3A1BF50-0BC7-1141-AFC5-6E9E0F0C2A71}">
+    <comment ref="B17" authorId="0" shapeId="0" xr:uid="{3918FDDB-A3E4-0B49-9E30-91DC8C33B5FA}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Should be 2019-03-31 00:00 according to Ray’s table, but I need a scale conversion factor for CSIRO-04 to WMO-2014XA?</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={2BCC7ABD-423F-9140-9F0E-0D3D48BA0BB7}</author>
+    <author>tc={9968C867-5802-9A4B-A2DE-541B0DFAE444}</author>
+  </authors>
+  <commentList>
+    <comment ref="B25" authorId="0" shapeId="0" xr:uid="{2BCC7ABD-423F-9140-9F0E-0D3D48BA0BB7}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Removed because I don’t know cal scale</t>
+      </text>
+    </comment>
+    <comment ref="D25" authorId="1" shapeId="0" xr:uid="{9968C867-5802-9A4B-A2DE-541B0DFAE444}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Flagged because I don’t know cal scale</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={4A039285-96F9-4143-A88F-8C916EDC0AD9}</author>
+    <author>tc={93EFDD1F-5B4C-C447-BA1B-4CBE61F64A50}</author>
+    <author>tc={20C96175-6992-8D40-9CA4-4CC3E72DCE98}</author>
+    <author>tc={E3A1BF50-0BC7-1141-AFC5-6E9E0F0C2A71}</author>
+    <author>tc={5C0CB34F-CFD5-784B-B25C-DBC14A041E76}</author>
+    <author>tc={4E5E7B0D-B6A0-8246-B428-30A869DD781A}</author>
+    <author>tc={18A65550-CF8C-E549-80FA-0DAEB7BD80E9}</author>
+    <author>tc={63DBE61C-638E-1240-8046-EAC6C26078CF}</author>
+  </authors>
+  <commentList>
+    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{4A039285-96F9-4143-A88F-8C916EDC0AD9}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Removed, because no cal scale in file</t>
+      </text>
+    </comment>
+    <comment ref="C9" authorId="1" shapeId="0" xr:uid="{93EFDD1F-5B4C-C447-BA1B-4CBE61F64A50}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Removed because no cal scale in file</t>
+      </text>
+    </comment>
+    <comment ref="B10" authorId="2" shapeId="0" xr:uid="{20C96175-6992-8D40-9CA4-4CC3E72DCE98}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Omitting because scale is not in file</t>
+      </text>
+    </comment>
+    <comment ref="C10" authorId="3" shapeId="0" xr:uid="{E3A1BF50-0BC7-1141-AFC5-6E9E0F0C2A71}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -58,7 +133,15 @@
     Omitting for now, because there’s no scale information in the THD files</t>
       </text>
     </comment>
-    <comment ref="B12" authorId="1" shapeId="0" xr:uid="{4E5E7B0D-B6A0-8246-B428-30A869DD781A}">
+    <comment ref="E11" authorId="4" shapeId="0" xr:uid="{5C0CB34F-CFD5-784B-B25C-DBC14A041E76}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Need to figure out how to deal with N2O scales</t>
+      </text>
+    </comment>
+    <comment ref="B12" authorId="5" shapeId="0" xr:uid="{4E5E7B0D-B6A0-8246-B428-30A869DD781A}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -66,12 +149,28 @@
     Removing this for now, because I can’t handle having the same species on two different Picarros</t>
       </text>
     </comment>
+    <comment ref="C12" authorId="6" shapeId="0" xr:uid="{18A65550-CF8C-E549-80FA-0DAEB7BD80E9}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Excluded because no scale information in file</t>
+      </text>
+    </comment>
+    <comment ref="E12" authorId="7" shapeId="0" xr:uid="{63DBE61C-638E-1240-8046-EAC6C26078CF}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Need to figure out how to convert scales</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="87">
   <si>
     <t>MHD</t>
   </si>
@@ -118,9 +217,6 @@
     <t>2017-02-15 00:00</t>
   </si>
   <si>
-    <t>2019-03-31 00:00</t>
-  </si>
-  <si>
     <t>x</t>
   </si>
   <si>
@@ -310,15 +406,6 @@
     <t>nf3</t>
   </si>
   <si>
-    <t>pfc-116</t>
-  </si>
-  <si>
-    <t>pfc-218</t>
-  </si>
-  <si>
-    <t>pfc-318</t>
-  </si>
-  <si>
     <t>h-2402</t>
   </si>
   <si>
@@ -335,13 +422,22 @@
   </si>
   <si>
     <t>cf4</t>
+  </si>
+  <si>
+    <t>c2f6</t>
+  </si>
+  <si>
+    <t>c3f8</t>
+  </si>
+  <si>
+    <t>c4f8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -380,6 +476,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -845,11 +947,48 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="B17" dT="2023-08-16T15:26:57.50" personId="{60FAC528-71CC-9C47-92F6-AF7323BA56B4}" id="{3918FDDB-A3E4-0B49-9E30-91DC8C33B5FA}">
+    <text>Should be 2019-03-31 00:00 according to Ray’s table, but I need a scale conversion factor for CSIRO-04 to WMO-2014XA?</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
+<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="B25" dT="2023-08-16T19:46:02.45" personId="{60FAC528-71CC-9C47-92F6-AF7323BA56B4}" id="{2BCC7ABD-423F-9140-9F0E-0D3D48BA0BB7}">
+    <text>Removed because I don’t know cal scale</text>
+  </threadedComment>
+  <threadedComment ref="D25" dT="2023-08-16T19:46:20.24" personId="{60FAC528-71CC-9C47-92F6-AF7323BA56B4}" id="{9968C867-5802-9A4B-A2DE-541B0DFAE444}">
+    <text>Flagged because I don’t know cal scale</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
+<file path=xl/threadedComments/threadedComment3.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="B9" dT="2023-08-16T23:43:54.87" personId="{60FAC528-71CC-9C47-92F6-AF7323BA56B4}" id="{4A039285-96F9-4143-A88F-8C916EDC0AD9}">
+    <text>Removed, because no cal scale in file</text>
+  </threadedComment>
+  <threadedComment ref="C9" dT="2023-08-16T23:44:48.21" personId="{60FAC528-71CC-9C47-92F6-AF7323BA56B4}" id="{93EFDD1F-5B4C-C447-BA1B-4CBE61F64A50}">
+    <text>Removed because no cal scale in file</text>
+  </threadedComment>
+  <threadedComment ref="B10" dT="2023-08-16T23:55:29.70" personId="{60FAC528-71CC-9C47-92F6-AF7323BA56B4}" id="{20C96175-6992-8D40-9CA4-4CC3E72DCE98}">
+    <text>Omitting because scale is not in file</text>
+  </threadedComment>
   <threadedComment ref="C10" dT="2023-08-03T19:14:34.78" personId="{60FAC528-71CC-9C47-92F6-AF7323BA56B4}" id="{E3A1BF50-0BC7-1141-AFC5-6E9E0F0C2A71}">
     <text>Omitting for now, because there’s no scale information in the THD files</text>
   </threadedComment>
+  <threadedComment ref="E11" dT="2023-08-17T10:12:40.61" personId="{60FAC528-71CC-9C47-92F6-AF7323BA56B4}" id="{5C0CB34F-CFD5-784B-B25C-DBC14A041E76}">
+    <text>Need to figure out how to deal with N2O scales</text>
+  </threadedComment>
   <threadedComment ref="B12" dT="2023-07-28T09:57:58.28" personId="{60FAC528-71CC-9C47-92F6-AF7323BA56B4}" id="{4E5E7B0D-B6A0-8246-B428-30A869DD781A}">
     <text>Removing this for now, because I can’t handle having the same species on two different Picarros</text>
+  </threadedComment>
+  <threadedComment ref="C12" dT="2023-08-16T23:48:01.25" personId="{60FAC528-71CC-9C47-92F6-AF7323BA56B4}" id="{18A65550-CF8C-E549-80FA-0DAEB7BD80E9}">
+    <text>Excluded because no scale information in file</text>
+  </threadedComment>
+  <threadedComment ref="E12" dT="2023-08-17T10:13:28.52" personId="{60FAC528-71CC-9C47-92F6-AF7323BA56B4}" id="{63DBE61C-638E-1240-8046-EAC6C26078CF}">
+    <text>Need to figure out how to convert scales</text>
   </threadedComment>
 </ThreadedComments>
 </file>
@@ -872,51 +1011,51 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>2</v>
@@ -930,27 +1069,27 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -976,51 +1115,51 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>2</v>
@@ -1034,37 +1173,37 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B15" s="14"/>
     </row>
@@ -1074,11 +1213,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F54C872C-8629-284F-A579-6B1D027BD782}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F54C872C-8629-284F-A579-6B1D027BD782}">
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView zoomScale="114" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1091,45 +1230,45 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>0</v>
@@ -1149,7 +1288,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>5</v>
@@ -1157,7 +1296,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>5</v>
@@ -1165,7 +1304,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>10</v>
@@ -1185,7 +1324,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>6</v>
@@ -1202,7 +1341,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>5</v>
@@ -1210,7 +1349,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>5</v>
@@ -1218,7 +1357,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>14</v>
@@ -1229,7 +1368,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>5</v>
@@ -1237,40 +1376,41 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1290,45 +1430,45 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>4</v>
@@ -1336,10 +1476,10 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1348,11 +1488,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6FA9302-AF76-F94F-9FFA-EB8BA8CE81F0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6FA9302-AF76-F94F-9FFA-EB8BA8CE81F0}">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1364,45 +1504,45 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>0</v>
@@ -1411,32 +1551,32 @@
         <v>4</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B10" s="12"/>
       <c r="C10" s="8"/>
@@ -1445,7 +1585,7 @@
     </row>
     <row r="11" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="8"/>
@@ -1454,7 +1594,7 @@
     </row>
     <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B12" s="12"/>
       <c r="C12" s="8"/>
@@ -1463,7 +1603,7 @@
     </row>
     <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="8"/>
@@ -1472,18 +1612,18 @@
     </row>
     <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B14" s="12"/>
       <c r="C14" s="8"/>
       <c r="D14" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E14" s="8"/>
     </row>
     <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B15" s="12"/>
       <c r="C15" s="8"/>
@@ -1492,35 +1632,35 @@
     </row>
     <row r="16" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B16" s="12"/>
       <c r="C16" s="8"/>
       <c r="D16" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E16" s="8"/>
     </row>
     <row r="17" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="8"/>
@@ -1529,7 +1669,7 @@
     </row>
     <row r="19" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B19" s="12"/>
       <c r="C19" s="8"/>
@@ -1538,7 +1678,7 @@
     </row>
     <row r="20" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B20" s="12"/>
       <c r="C20" s="8"/>
@@ -1547,7 +1687,7 @@
     </row>
     <row r="21" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B21" s="12"/>
       <c r="C21" s="8"/>
@@ -1556,7 +1696,7 @@
     </row>
     <row r="22" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B22" s="12"/>
       <c r="C22" s="8"/>
@@ -1565,7 +1705,7 @@
     </row>
     <row r="23" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="8"/>
@@ -1574,90 +1714,95 @@
     </row>
     <row r="24" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
     </row>
     <row r="25" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B25" s="12"/>
+        <v>51</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>15</v>
+      </c>
       <c r="C25" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D25" s="8"/>
+        <v>15</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>15</v>
+      </c>
       <c r="E25" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B26" s="12"/>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
       <c r="E26" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D27" s="8"/>
       <c r="E27" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D29" s="8"/>
       <c r="E29" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1665,8 +1810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DC23F92-7B72-094D-8D01-143767015082}">
   <dimension ref="A1:B49"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" zoomScale="116" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+    <sheetView zoomScale="116" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1678,315 +1823,315 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B10" s="22"/>
     </row>
     <row r="11" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B11" s="22"/>
     </row>
     <row r="12" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B12" s="22"/>
     </row>
     <row r="13" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B13" s="22"/>
     </row>
     <row r="14" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B14" s="22"/>
     </row>
     <row r="15" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B15" s="22"/>
     </row>
     <row r="16" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B16" s="23"/>
     </row>
     <row r="17" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B17" s="22"/>
     </row>
     <row r="18" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B18" s="22"/>
     </row>
     <row r="19" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B19" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B20" s="24"/>
     </row>
     <row r="21" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B21" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B22" s="24"/>
     </row>
     <row r="23" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B23" s="24"/>
     </row>
     <row r="24" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B24" s="24"/>
     </row>
     <row r="25" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B25" s="24"/>
     </row>
     <row r="26" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B26" s="24"/>
     </row>
     <row r="27" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B27" s="24"/>
     </row>
     <row r="28" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B28" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B29" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B30" s="25"/>
     </row>
     <row r="31" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B31" s="25"/>
     </row>
     <row r="32" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B32" s="24"/>
     </row>
     <row r="33" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B33" s="24"/>
     </row>
     <row r="34" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="16" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B34" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B35" s="24"/>
     </row>
     <row r="36" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B36" s="24"/>
     </row>
     <row r="37" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B37" s="24"/>
     </row>
     <row r="38" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B38" s="24"/>
     </row>
     <row r="39" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B39" s="24"/>
     </row>
     <row r="40" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B40" s="24"/>
     </row>
     <row r="41" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B41" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B42" s="24"/>
     </row>
     <row r="43" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B43" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B44" s="24"/>
     </row>
     <row r="45" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B45" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="16" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B46" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="16" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="B47" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="16" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="B48" s="24"/>
     </row>
     <row r="49" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="16" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="B49" s="24"/>
     </row>
@@ -1999,8 +2144,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CEEAF2A-BA72-FC4F-92D8-D72395398919}">
   <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="75" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2012,45 +2157,45 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="19" t="s">
         <v>21</v>
-      </c>
-      <c r="B7" s="19" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" s="21" t="s">
         <v>0</v>
@@ -2068,21 +2213,21 @@
         <v>4</v>
       </c>
       <c r="G8" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H8" s="21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I8" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="J8" s="21" t="s">
         <v>59</v>
-      </c>
-      <c r="J8" s="21" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B9" s="22"/>
       <c r="C9" s="22"/>
@@ -2092,15 +2237,15 @@
       <c r="G9" s="22"/>
       <c r="H9" s="22"/>
       <c r="I9" s="23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J9" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B10" s="22"/>
       <c r="C10" s="23"/>
@@ -2111,12 +2256,12 @@
       <c r="H10" s="22"/>
       <c r="I10" s="22"/>
       <c r="J10" s="23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B11" s="22"/>
       <c r="C11" s="23"/>
@@ -2127,12 +2272,12 @@
       <c r="H11" s="22"/>
       <c r="I11" s="22"/>
       <c r="J11" s="23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B12" s="22"/>
       <c r="C12" s="22"/>
@@ -2143,12 +2288,12 @@
       <c r="H12" s="22"/>
       <c r="I12" s="22"/>
       <c r="J12" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B13" s="22"/>
       <c r="C13" s="22"/>
@@ -2159,12 +2304,12 @@
       <c r="H13" s="22"/>
       <c r="I13" s="22"/>
       <c r="J13" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B14" s="22"/>
       <c r="C14" s="22"/>
@@ -2175,12 +2320,12 @@
       <c r="H14" s="22"/>
       <c r="I14" s="22"/>
       <c r="J14" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B15" s="22"/>
       <c r="C15" s="22"/>
@@ -2191,12 +2336,12 @@
       <c r="H15" s="22"/>
       <c r="I15" s="22"/>
       <c r="J15" s="23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B16" s="22"/>
       <c r="C16" s="22"/>
@@ -2207,12 +2352,12 @@
       <c r="H16" s="22"/>
       <c r="I16" s="23"/>
       <c r="J16" s="23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B17" s="22"/>
       <c r="C17" s="22"/>
@@ -2223,12 +2368,12 @@
       <c r="H17" s="22"/>
       <c r="I17" s="22"/>
       <c r="J17" s="23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B18" s="22"/>
       <c r="C18" s="22"/>
@@ -2239,12 +2384,12 @@
       <c r="H18" s="22"/>
       <c r="I18" s="22"/>
       <c r="J18" s="23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B19" s="24"/>
       <c r="C19" s="24"/>
@@ -2254,15 +2399,15 @@
       <c r="G19" s="24"/>
       <c r="H19" s="24"/>
       <c r="I19" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J19" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B20" s="24"/>
       <c r="C20" s="24"/>
@@ -2271,16 +2416,16 @@
       <c r="F20" s="24"/>
       <c r="G20" s="25"/>
       <c r="H20" s="23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I20" s="24"/>
       <c r="J20" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B21" s="24"/>
       <c r="C21" s="24"/>
@@ -2290,15 +2435,15 @@
       <c r="G21" s="24"/>
       <c r="H21" s="24"/>
       <c r="I21" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J21" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B22" s="24"/>
       <c r="C22" s="24"/>
@@ -2309,12 +2454,12 @@
       <c r="H22" s="24"/>
       <c r="I22" s="24"/>
       <c r="J22" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B23" s="24"/>
       <c r="C23" s="24"/>
@@ -2325,12 +2470,12 @@
       <c r="H23" s="24"/>
       <c r="I23" s="24"/>
       <c r="J23" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B24" s="24"/>
       <c r="C24" s="24"/>
@@ -2341,12 +2486,12 @@
       <c r="H24" s="24"/>
       <c r="I24" s="24"/>
       <c r="J24" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B25" s="24"/>
       <c r="C25" s="24"/>
@@ -2357,64 +2502,64 @@
       <c r="H25" s="24"/>
       <c r="I25" s="24"/>
       <c r="J25" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B26" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C26" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D26" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E26" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F26" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G26" s="24"/>
       <c r="H26" s="24"/>
       <c r="I26" s="24"/>
       <c r="J26" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B27" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D27" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E27" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F27" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G27" s="24"/>
       <c r="H27" s="24"/>
       <c r="I27" s="24"/>
       <c r="J27" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B28" s="24"/>
       <c r="C28" s="24"/>
@@ -2424,15 +2569,15 @@
       <c r="G28" s="24"/>
       <c r="H28" s="24"/>
       <c r="I28" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J28" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B29" s="24"/>
       <c r="C29" s="24"/>
@@ -2442,15 +2587,15 @@
       <c r="G29" s="24"/>
       <c r="H29" s="24"/>
       <c r="I29" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J29" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B30" s="24"/>
       <c r="C30" s="24"/>
@@ -2461,12 +2606,12 @@
       <c r="H30" s="24"/>
       <c r="I30" s="25"/>
       <c r="J30" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B31" s="24"/>
       <c r="C31" s="24"/>
@@ -2477,12 +2622,12 @@
       <c r="H31" s="24"/>
       <c r="I31" s="25"/>
       <c r="J31" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B32" s="24"/>
       <c r="C32" s="24"/>
@@ -2493,12 +2638,12 @@
       <c r="H32" s="24"/>
       <c r="I32" s="24"/>
       <c r="J32" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B33" s="24"/>
       <c r="C33" s="24"/>
@@ -2509,12 +2654,12 @@
       <c r="H33" s="24"/>
       <c r="I33" s="24"/>
       <c r="J33" s="23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="16" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B34" s="24"/>
       <c r="C34" s="24"/>
@@ -2524,15 +2669,15 @@
       <c r="G34" s="24"/>
       <c r="H34" s="24"/>
       <c r="I34" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J34" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B35" s="24"/>
       <c r="C35" s="24"/>
@@ -2543,12 +2688,12 @@
       <c r="H35" s="24"/>
       <c r="I35" s="24"/>
       <c r="J35" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B36" s="24"/>
       <c r="C36" s="24"/>
@@ -2559,15 +2704,15 @@
       <c r="H36" s="24"/>
       <c r="I36" s="24"/>
       <c r="J36" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B37" s="23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C37" s="24"/>
       <c r="D37" s="24"/>
@@ -2577,15 +2722,15 @@
       <c r="H37" s="24"/>
       <c r="I37" s="24"/>
       <c r="J37" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B38" s="23" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C38" s="24"/>
       <c r="D38" s="24"/>
@@ -2595,12 +2740,12 @@
       <c r="H38" s="24"/>
       <c r="I38" s="24"/>
       <c r="J38" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B39" s="24"/>
       <c r="C39" s="24"/>
@@ -2611,72 +2756,72 @@
       <c r="H39" s="24"/>
       <c r="I39" s="24"/>
       <c r="J39" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B40" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C40" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D40" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E40" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F40" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G40" s="24"/>
       <c r="H40" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I40" s="24"/>
       <c r="J40" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B41" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C41" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D41" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E41" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F41" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G41" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H41" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I41" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J41" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B42" s="24"/>
       <c r="C42" s="24"/>
@@ -2687,12 +2832,12 @@
       <c r="H42" s="24"/>
       <c r="I42" s="24"/>
       <c r="J42" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B43" s="24"/>
       <c r="C43" s="24"/>
@@ -2702,15 +2847,15 @@
       <c r="G43" s="24"/>
       <c r="H43" s="24"/>
       <c r="I43" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J43" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B44" s="24"/>
       <c r="C44" s="24"/>
@@ -2721,12 +2866,12 @@
       <c r="H44" s="24"/>
       <c r="I44" s="24"/>
       <c r="J44" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B45" s="24"/>
       <c r="C45" s="24"/>
@@ -2736,15 +2881,15 @@
       <c r="G45" s="24"/>
       <c r="H45" s="24"/>
       <c r="I45" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J45" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="16" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B46" s="24"/>
       <c r="C46" s="24"/>
@@ -2754,15 +2899,15 @@
       <c r="G46" s="24"/>
       <c r="H46" s="24"/>
       <c r="I46" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J46" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="16" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="B47" s="24"/>
       <c r="C47" s="24"/>
@@ -2772,15 +2917,15 @@
       <c r="G47" s="24"/>
       <c r="H47" s="24"/>
       <c r="I47" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J47" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="16" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="B48" s="24"/>
       <c r="C48" s="24"/>
@@ -2791,12 +2936,12 @@
       <c r="H48" s="24"/>
       <c r="I48" s="24"/>
       <c r="J48" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="16" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="B49" s="24"/>
       <c r="C49" s="24"/>
@@ -2807,7 +2952,7 @@
       <c r="H49" s="24"/>
       <c r="I49" s="24"/>
       <c r="J49" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -2831,45 +2976,45 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>4</v>
@@ -2877,7 +3022,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -2890,7 +3035,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2902,48 +3047,48 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>1</v>
@@ -2957,54 +3102,72 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>85</v>
+        <v>81</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>